<commit_message>
finish import from excel
</commit_message>
<xml_diff>
--- a/public/myusers.xlsx
+++ b/public/myusers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marwa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F112323-6F38-41BB-A97C-AB2B18C9D4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{985B5962-C171-4332-B5B4-24C9C919B893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0C55E41B-5A66-4DCA-AA36-851E2D8A95DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FE60CA0-CE63-4AA0-8591-869F682C2CA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,73 +35,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Created At</t>
-  </si>
-  <si>
-    <t>Updated At</t>
-  </si>
-  <si>
-    <t>noor</t>
+    <t>Noor</t>
   </si>
   <si>
     <t>noor@noor.com</t>
   </si>
   <si>
-    <t>naser</t>
-  </si>
-  <si>
-    <t>naser@naser.com</t>
-  </si>
-  <si>
-    <t>salim</t>
-  </si>
-  <si>
-    <t>salim@salim.com</t>
-  </si>
-  <si>
     <t>Noo12345678</t>
-  </si>
-  <si>
-    <t>Nas12345678</t>
-  </si>
-  <si>
-    <t>Sal12345678</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFA31515"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <u/>
@@ -131,14 +86,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -453,96 +405,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A5A59A-A46E-4215-9EB6-7BFBCFD23E23}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A651EB8C-0D40-4267-BFE0-B8BC27086957}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
+      <c r="D1">
         <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{078F7EEE-DDAF-4F3E-9022-3F1EFCDF6586}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{109E64F1-6A4B-46CC-8A0A-633C49D9FF35}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{366A86B3-F394-4FE3-9DA6-D5EFF8B397B2}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{03B3DAAB-36FC-4F5A-AF9E-F90AE25549BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>